<commit_message>
added min/max and other details
</commit_message>
<xml_diff>
--- a/Feather-sensor-testing/meganSensorTesting1.xlsx
+++ b/Feather-sensor-testing/meganSensorTesting1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EC19EA6-7BF0-46B0-9F80-AADB992E5C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705FC938-8A90-4F49-B3E9-949B8F7D7D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{D615EB67-25BF-45D8-A251-24551AE9CFE9}"/>
   </bookViews>
@@ -5309,6 +5309,359 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>105834</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>58795</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>352779</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>105834</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FE0478A-7CDE-1735-6EEF-AECDC3C3B6A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8055093" y="811388"/>
+          <a:ext cx="2692871" cy="1175927"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Sensor 1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>max</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> val - 30983</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>min val - 19668</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>This sensor appears to not be working properly, with a random jump 4 hours into testing.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>47037</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>70556</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>305741</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152871</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F6908E3-0994-CFCE-DEEF-2F0A06D83F36}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7996296" y="70556"/>
+          <a:ext cx="2704630" cy="646759"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>disclaimer:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> I watered the dirt before putting the sensors in, so the max value shown is likely not the max value of the sensor</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>105834</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>176389</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>341019</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>11759</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CAD0E0D-B127-3B3D-4B95-01A8C575AF98}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8055093" y="2057870"/>
+          <a:ext cx="2681111" cy="1152408"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Sensor 2</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>max val - 21669</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>min val - 21045</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Seems</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> to be working fine for the most part. There is a random jump but there still seems to be a steady upward trend.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>105834</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>105833</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>176389</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C78CD4BD-A4D3-7D4A-8C78-BFEA4A05B31D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8055093" y="3304352"/>
+          <a:ext cx="2657592" cy="823148"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Sensor 3</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>max</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> val - 20468</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>min val - 20164</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Working great!</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5632,7 +5985,7 @@
   <dimension ref="A1:D100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="54" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>